<commit_message>
Cuda Tearing PARTIALLY Fixed
</commit_message>
<xml_diff>
--- a/Benchmark Visuals.xlsx
+++ b/Benchmark Visuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blcag\Documents\CMU Spring 2023 Folder\Animation\Final\AMCViewer-simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C9331E-FDA4-4CFF-A97B-0F9505F0475A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB03951-A652-46F7-9FE5-3D28A3615AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,10 +162,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14160,8 +14159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14315,19 +14314,19 @@
       <c r="I25" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25">
         <v>2.9832946557127098</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25">
         <v>6.9075654961593003</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25">
         <v>13.5565045427188</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25">
         <v>19.164741750804101</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25">
         <v>27.911772930648802</v>
       </c>
     </row>
@@ -14413,19 +14412,19 @@
       <c r="I48" t="s">
         <v>20</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48">
         <v>3.35698295723786</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48">
         <v>7.7299048953642897</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48">
         <v>28.095122750523601</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48">
         <v>121.34793974983501</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48">
         <v>555.60419100579804</v>
       </c>
     </row>
@@ -14511,19 +14510,19 @@
       <c r="I68" t="s">
         <v>20</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68">
         <v>65.202547289642595</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68">
         <v>258.91343447296902</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68">
         <v>921.60257112596298</v>
       </c>
-      <c r="M68" s="2">
+      <c r="M68">
         <v>4244.4476914085299</v>
       </c>
-      <c r="N68" s="2">
+      <c r="N68">
         <v>20842.451395454002</v>
       </c>
     </row>
@@ -14609,19 +14608,19 @@
       <c r="I88" t="s">
         <v>20</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88">
         <v>3.5737254013490301</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88">
         <v>20.873922434762299</v>
       </c>
-      <c r="L88" s="2">
+      <c r="L88">
         <v>74.177766939982305</v>
       </c>
-      <c r="M88" s="2">
+      <c r="M88">
         <v>349.54626125975301</v>
       </c>
-      <c r="N88" s="2">
+      <c r="N88">
         <v>1592.39261680136</v>
       </c>
     </row>
@@ -14829,43 +14828,43 @@
       <c r="A130" t="s">
         <v>25</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130">
         <v>58.091575559712297</v>
       </c>
-      <c r="C130" s="2">
+      <c r="C130">
         <v>58.0420108074224</v>
       </c>
-      <c r="D130" s="2">
+      <c r="D130">
         <v>34.017539443337</v>
       </c>
-      <c r="E130" s="2">
+      <c r="E130">
         <v>8.6544120192474097</v>
       </c>
-      <c r="F130" s="2">
+      <c r="F130">
         <v>3.59547976284215</v>
       </c>
-      <c r="G130" s="2">
+      <c r="G130">
         <v>2.1356341231620202</v>
       </c>
       <c r="I130" t="s">
         <v>25</v>
       </c>
-      <c r="J130" s="2">
+      <c r="J130">
         <v>57.577816418890102</v>
       </c>
-      <c r="K130" s="2">
+      <c r="K130">
         <v>57.505635552284097</v>
       </c>
-      <c r="L130" s="2">
+      <c r="L130">
         <v>57.248193819485003</v>
       </c>
-      <c r="M130" s="2">
+      <c r="M130">
         <v>56.710882251195201</v>
       </c>
-      <c r="N130" s="2">
+      <c r="N130">
         <v>55.282521325232601</v>
       </c>
-      <c r="O130" s="2">
+      <c r="O130">
         <v>42.8617964236117</v>
       </c>
     </row>
@@ -14873,43 +14872,43 @@
       <c r="A131" t="s">
         <v>17</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131">
         <v>58.710942545471603</v>
       </c>
-      <c r="C131" s="2">
+      <c r="C131">
         <v>58.550066161574797</v>
       </c>
-      <c r="D131" s="2">
+      <c r="D131">
         <v>23.231393976564199</v>
       </c>
-      <c r="E131" s="2">
+      <c r="E131">
         <v>4.91045780198088</v>
       </c>
-      <c r="F131" s="2">
+      <c r="F131">
         <v>2.2238876669861698</v>
       </c>
-      <c r="G131" s="2">
+      <c r="G131">
         <v>1.1789408159921</v>
       </c>
       <c r="I131" t="s">
         <v>17</v>
       </c>
-      <c r="J131" s="2">
+      <c r="J131">
         <v>58.235013219347998</v>
       </c>
-      <c r="K131" s="2">
+      <c r="K131">
         <v>58.504165496583397</v>
       </c>
-      <c r="L131" s="2">
+      <c r="L131">
         <v>45.651469292539197</v>
       </c>
-      <c r="M131" s="2">
+      <c r="M131">
         <v>11.7813661200898</v>
       </c>
-      <c r="N131" s="2">
+      <c r="N131">
         <v>4.8461352071722796</v>
       </c>
-      <c r="O131" s="2">
+      <c r="O131">
         <v>2.9754731746215901</v>
       </c>
     </row>

</xml_diff>